<commit_message>
add gene noncoding and sliding/dynamic window
</commit_message>
<xml_diff>
--- a/inst/extdata/HDL_C.xlsx
+++ b/inst/extdata/HDL_C.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://indiana-my.sharepoint.com/personal/yzh10_iu_edu/Documents/research/nuMoM2b/whole_sequencing/for_use/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://indiana-my.sharepoint.com/personal/yzh10_iu_edu/Documents/research/nuMoM2b/whole_sequencing/mr.carv/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="8_{EB338793-E911-CF44-9B38-94A76EF1FAB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26829451-DAB1-134D-81DC-493B6D52C5E5}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="8_{EB338793-E911-CF44-9B38-94A76EF1FAB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23E207FB-20EC-7F40-8F77-94DEF4FEF382}"/>
   <bookViews>
-    <workbookView xWindow="54160" yWindow="2460" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{8CF3AADF-3B51-1B4F-985A-713C56632C1E}"/>
+    <workbookView xWindow="38400" yWindow="2720" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{8CF3AADF-3B51-1B4F-985A-713C56632C1E}"/>
   </bookViews>
   <sheets>
     <sheet name="indv_effect" sheetId="1" r:id="rId1"/>
-    <sheet name="gene_effect" sheetId="2" r:id="rId2"/>
+    <sheet name="coding" sheetId="2" r:id="rId2"/>
+    <sheet name="noncoding" sheetId="3" r:id="rId3"/>
+    <sheet name="window" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2185" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2285" uniqueCount="513">
   <si>
     <t>A</t>
   </si>
@@ -1504,6 +1506,78 @@
   </si>
   <si>
     <t>disruptive_missense</t>
+  </si>
+  <si>
+    <t>UTR</t>
+  </si>
+  <si>
+    <t>rs34498052</t>
+  </si>
+  <si>
+    <t>rs34498052, rs34119551</t>
+  </si>
+  <si>
+    <t>GFOD2</t>
+  </si>
+  <si>
+    <t>promoter_CAGE</t>
+  </si>
+  <si>
+    <t>enhancer_DHS</t>
+  </si>
+  <si>
+    <t>promoter_DHS</t>
+  </si>
+  <si>
+    <t>enhancer_CAGE</t>
+  </si>
+  <si>
+    <t>Start.Loc</t>
+  </si>
+  <si>
+    <t>End.Loc</t>
+  </si>
+  <si>
+    <t>Genes linked to the region</t>
+  </si>
+  <si>
+    <t>Regions (regulatory element in the region)</t>
+  </si>
+  <si>
+    <t>UTR-Exon1-Intron1(EH38E1818390 proximal enhancer like signature, EH38E1818391 proximal enhancer like signature)</t>
+  </si>
+  <si>
+    <t>UTR-Exon1-Intron1-Exon2-Intron2-Exon3-Intron3 (EH38E1572746 promoter like signature, EH38E1572747 proximal enhancer like signature)</t>
+  </si>
+  <si>
+    <t>Exon2-Intron2-Exon3-Intron3 (EH38E1572747 proximal enhancer like signature), EH38E1572749 proximal enhancer like signature), EH38E1572750 proximal enhancer like signature)</t>
+  </si>
+  <si>
+    <t>Exon6 (EH38E1823417 distal enhancer like signature)</t>
+  </si>
+  <si>
+    <t>Exon2-Intron2-Exon3-Intron3 (EH38E1572747 proximal enhancer like signature)</t>
+  </si>
+  <si>
+    <t>Intron7-Exon7 (EH38E2713970  distal enhancer like signature)</t>
+  </si>
+  <si>
+    <t>Intron7-Exon7 (EH38E2713970 distal enhancer like signature)</t>
+  </si>
+  <si>
+    <t>Intron24-Exon25-Intron25-Exon26-Intron26 (EH38E1818501 distal enhancer like signature)</t>
+  </si>
+  <si>
+    <t>LPL (near by gene)</t>
+  </si>
+  <si>
+    <t>Intron4</t>
+  </si>
+  <si>
+    <t>LCAT; SLC12A4</t>
+  </si>
+  <si>
+    <t>Exon3-Intron2-Exon2-Intron1; Exon24 (EH38E1823423 proximal enhancer like signature, EH38E1823424 proximal enhancer like signature)</t>
   </si>
 </sst>
 </file>
@@ -1513,7 +1587,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1578,6 +1652,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1587,7 +1667,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1699,11 +1779,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1802,6 +1944,112 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2142,7 +2390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{507F472E-772F-E949-B612-5FED0D7A26C2}">
   <dimension ref="A1:L358"/>
   <sheetViews>
-    <sheetView topLeftCell="A327" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:L358"/>
     </sheetView>
   </sheetViews>
@@ -15614,8 +15862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85D427D3-02D1-0F48-84C3-582D66EA14C9}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16757,4 +17005,1016 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9452BA7A-DAEC-8445-BDD5-0FF92B0E6218}">
+  <dimension ref="A1:O11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="N1" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="13">
+        <v>16</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>490</v>
+      </c>
+      <c r="F2" s="13">
+        <v>82</v>
+      </c>
+      <c r="G2" s="14">
+        <v>4.6059999999999998E-7</v>
+      </c>
+      <c r="H2" s="14">
+        <v>2.0990000000000001E-6</v>
+      </c>
+      <c r="I2" s="14">
+        <v>6.6309999999999995E-7</v>
+      </c>
+      <c r="J2" s="14">
+        <v>3.3649999999999998E-7</v>
+      </c>
+      <c r="K2" s="40">
+        <v>1.0976634505427101</v>
+      </c>
+      <c r="L2">
+        <v>0.46111878523114302</v>
+      </c>
+      <c r="M2" s="41">
+        <v>1.7292195691798601E-2</v>
+      </c>
+      <c r="N2" s="16">
+        <v>64</v>
+      </c>
+      <c r="O2" s="17">
+        <v>0.190049226653078</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="19">
+        <v>11</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>493</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="19">
+        <v>238</v>
+      </c>
+      <c r="G3" s="20">
+        <v>5.687E-4</v>
+      </c>
+      <c r="H3" s="20">
+        <v>1.829E-7</v>
+      </c>
+      <c r="I3" s="20">
+        <v>2.796E-5</v>
+      </c>
+      <c r="J3" s="20">
+        <v>6.286E-7</v>
+      </c>
+      <c r="K3" s="3">
+        <v>-1.45056390909559</v>
+      </c>
+      <c r="L3">
+        <v>0.269541795479113</v>
+      </c>
+      <c r="M3" s="4">
+        <v>7.3830046570049496E-8</v>
+      </c>
+      <c r="N3" s="22">
+        <v>195</v>
+      </c>
+      <c r="O3" s="23">
+        <v>2.3225833367668301E-8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="19">
+        <v>11</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>493</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="19">
+        <v>114</v>
+      </c>
+      <c r="G4" s="20">
+        <v>0.1416</v>
+      </c>
+      <c r="H4" s="20">
+        <v>0.4294</v>
+      </c>
+      <c r="I4" s="20">
+        <v>2.1959999999999998E-6</v>
+      </c>
+      <c r="J4" s="20">
+        <v>5.7760000000000003E-6</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.514393377210558</v>
+      </c>
+      <c r="L4">
+        <v>0.42551374068549602</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0.226710462183007</v>
+      </c>
+      <c r="N4" s="22">
+        <v>83</v>
+      </c>
+      <c r="O4" s="23">
+        <v>0.20465913683515999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="19">
+        <v>16</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>494</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>491</v>
+      </c>
+      <c r="F5" s="19">
+        <v>548</v>
+      </c>
+      <c r="G5" s="20">
+        <v>1.044E-4</v>
+      </c>
+      <c r="H5" s="20">
+        <v>0.1489</v>
+      </c>
+      <c r="I5" s="20">
+        <v>8.3189999999999995E-6</v>
+      </c>
+      <c r="J5" s="20">
+        <v>6.5209999999999999E-6</v>
+      </c>
+      <c r="K5" s="3">
+        <v>-7.9803189537385605E-2</v>
+      </c>
+      <c r="L5">
+        <v>0.165404805606443</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0.62947067512336696</v>
+      </c>
+      <c r="N5" s="22">
+        <v>402</v>
+      </c>
+      <c r="O5" s="23">
+        <v>6.4994896439163298E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="19">
+        <v>16</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>495</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>491</v>
+      </c>
+      <c r="F6" s="19">
+        <v>416</v>
+      </c>
+      <c r="G6" s="20">
+        <v>4.5320000000000001E-4</v>
+      </c>
+      <c r="H6" s="20">
+        <v>1.304E-2</v>
+      </c>
+      <c r="I6" s="20">
+        <v>4.4399999999999998E-6</v>
+      </c>
+      <c r="J6" s="20">
+        <v>1.2819999999999999E-5</v>
+      </c>
+      <c r="K6" s="3">
+        <v>-0.17092591137985899</v>
+      </c>
+      <c r="L6">
+        <v>0.21415948540763599</v>
+      </c>
+      <c r="M6" s="4">
+        <v>0.42479830158471199</v>
+      </c>
+      <c r="N6" s="22">
+        <v>280</v>
+      </c>
+      <c r="O6" s="23">
+        <v>4.9354982189987497E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="B7" s="19">
+        <v>16</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>494</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="19">
+        <v>2007</v>
+      </c>
+      <c r="G7" s="20">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="H7" s="20">
+        <v>0.24160000000000001</v>
+      </c>
+      <c r="I7" s="20">
+        <v>5.2660000000000001E-6</v>
+      </c>
+      <c r="J7" s="20">
+        <v>1.506E-5</v>
+      </c>
+      <c r="K7" s="3">
+        <v>-0.26525477325830299</v>
+      </c>
+      <c r="L7">
+        <v>0.12562178040845501</v>
+      </c>
+      <c r="M7" s="4">
+        <v>3.4726361611768099E-2</v>
+      </c>
+      <c r="N7" s="22">
+        <v>715</v>
+      </c>
+      <c r="O7" s="23">
+        <v>2.4881208204874399E-12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="19">
+        <v>11</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>495</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" s="19">
+        <v>459</v>
+      </c>
+      <c r="G8" s="20">
+        <v>0.251</v>
+      </c>
+      <c r="H8" s="20">
+        <v>0.54320000000000002</v>
+      </c>
+      <c r="I8" s="20">
+        <v>1.1759999999999999E-5</v>
+      </c>
+      <c r="J8" s="20">
+        <v>2.8160000000000001E-5</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.21558340104673701</v>
+      </c>
+      <c r="L8">
+        <v>0.19230804852168501</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0.26227440795350998</v>
+      </c>
+      <c r="N8" s="22">
+        <v>312</v>
+      </c>
+      <c r="O8" s="23">
+        <v>1.69142579865127E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="19">
+        <v>11</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>496</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="19">
+        <v>662</v>
+      </c>
+      <c r="G9" s="20">
+        <v>8.2190000000000006E-3</v>
+      </c>
+      <c r="H9" s="20">
+        <v>2.5579999999999999E-3</v>
+      </c>
+      <c r="I9" s="20">
+        <v>1.358E-5</v>
+      </c>
+      <c r="J9" s="20">
+        <v>3.6510000000000001E-5</v>
+      </c>
+      <c r="K9" s="3">
+        <v>-0.36145672044860899</v>
+      </c>
+      <c r="L9">
+        <v>0.17095529314100499</v>
+      </c>
+      <c r="M9" s="4">
+        <v>3.4486684628685503E-2</v>
+      </c>
+      <c r="N9" s="22">
+        <v>471</v>
+      </c>
+      <c r="O9" s="23">
+        <v>4.2033484914938399E-8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="19">
+        <v>11</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>494</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" s="19">
+        <v>3945</v>
+      </c>
+      <c r="G10" s="20">
+        <v>1.8839999999999999E-2</v>
+      </c>
+      <c r="H10" s="20">
+        <v>0.13639999999999999</v>
+      </c>
+      <c r="I10" s="20">
+        <v>7.6959999999999995E-5</v>
+      </c>
+      <c r="J10" s="20">
+        <v>1.8789999999999999E-4</v>
+      </c>
+      <c r="K10" s="3">
+        <v>-6.1380190147929696E-3</v>
+      </c>
+      <c r="L10">
+        <v>0.121267834893241</v>
+      </c>
+      <c r="M10" s="4">
+        <v>0.95963199740798</v>
+      </c>
+      <c r="N10" s="22">
+        <v>2108</v>
+      </c>
+      <c r="O10" s="23">
+        <v>3.5216274341110001E-13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>492</v>
+      </c>
+      <c r="B11" s="25">
+        <v>16</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>494</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="25">
+        <v>318</v>
+      </c>
+      <c r="G11" s="26">
+        <v>5.9380000000000001E-4</v>
+      </c>
+      <c r="H11" s="26">
+        <v>0.65190000000000003</v>
+      </c>
+      <c r="I11" s="26">
+        <v>7.2170000000000003E-3</v>
+      </c>
+      <c r="J11" s="26">
+        <v>2.0230000000000001E-3</v>
+      </c>
+      <c r="K11" s="34">
+        <v>0.11856336828047601</v>
+      </c>
+      <c r="L11">
+        <v>0.22223805796903301</v>
+      </c>
+      <c r="M11" s="35">
+        <v>0.59368949043151298</v>
+      </c>
+      <c r="N11" s="27">
+        <v>286</v>
+      </c>
+      <c r="O11" s="28">
+        <v>0.146015700509396</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DFAAA2-8957-BD49-9367-1B791D4363AF}">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1:L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="53.6640625" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
+    <col min="11" max="11" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="76" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="76" t="s">
+        <v>497</v>
+      </c>
+      <c r="C1" s="77" t="s">
+        <v>498</v>
+      </c>
+      <c r="D1" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="78" t="s">
+        <v>499</v>
+      </c>
+      <c r="F1" s="77" t="s">
+        <v>500</v>
+      </c>
+      <c r="G1" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="51">
+        <v>16</v>
+      </c>
+      <c r="B2" s="51">
+        <v>56961038</v>
+      </c>
+      <c r="C2" s="52">
+        <v>56963037</v>
+      </c>
+      <c r="D2" s="52">
+        <v>313</v>
+      </c>
+      <c r="E2" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="54" t="s">
+        <v>501</v>
+      </c>
+      <c r="G2" s="55">
+        <v>0.40013222034193202</v>
+      </c>
+      <c r="H2">
+        <v>0.23033197682103501</v>
+      </c>
+      <c r="I2" s="56">
+        <v>8.2352250146882994E-2</v>
+      </c>
+      <c r="J2" s="57">
+        <v>276</v>
+      </c>
+      <c r="K2" s="58">
+        <v>4.78499548704159E-4</v>
+      </c>
+      <c r="L2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="59">
+        <v>11</v>
+      </c>
+      <c r="B3" s="59">
+        <v>116829402</v>
+      </c>
+      <c r="C3" s="60">
+        <v>116831401</v>
+      </c>
+      <c r="D3" s="60">
+        <v>337</v>
+      </c>
+      <c r="E3" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="62" t="s">
+        <v>502</v>
+      </c>
+      <c r="G3" s="63">
+        <v>-8.8108351260473994E-3</v>
+      </c>
+      <c r="H3">
+        <v>0.25370124305486502</v>
+      </c>
+      <c r="I3" s="64">
+        <v>0.97229569585692799</v>
+      </c>
+      <c r="J3" s="65">
+        <v>275</v>
+      </c>
+      <c r="K3" s="66">
+        <v>1.0991207943788999E-14</v>
+      </c>
+      <c r="L3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="67">
+        <v>11</v>
+      </c>
+      <c r="B4" s="67">
+        <v>116830402</v>
+      </c>
+      <c r="C4" s="68">
+        <v>116832401</v>
+      </c>
+      <c r="D4" s="68">
+        <v>307</v>
+      </c>
+      <c r="E4" s="69" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="70" t="s">
+        <v>503</v>
+      </c>
+      <c r="G4" s="71">
+        <v>0.21567633653818499</v>
+      </c>
+      <c r="H4">
+        <v>0.2180057233123</v>
+      </c>
+      <c r="I4" s="72">
+        <v>0.32250903750351301</v>
+      </c>
+      <c r="J4" s="73">
+        <v>288</v>
+      </c>
+      <c r="K4" s="74">
+        <v>6.4690031109648797E-11</v>
+      </c>
+      <c r="L4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="51">
+        <v>16</v>
+      </c>
+      <c r="B5" s="51">
+        <v>67939898</v>
+      </c>
+      <c r="C5" s="52">
+        <v>67940531</v>
+      </c>
+      <c r="D5" s="51">
+        <v>90</v>
+      </c>
+      <c r="E5" s="79" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="80" t="s">
+        <v>504</v>
+      </c>
+      <c r="G5" s="84">
+        <v>-3.67774669551922</v>
+      </c>
+      <c r="H5">
+        <v>0.566847299554055</v>
+      </c>
+      <c r="I5" s="87">
+        <v>8.6941119210006803E-11</v>
+      </c>
+      <c r="J5" s="39">
+        <v>95</v>
+      </c>
+      <c r="K5" s="17">
+        <v>2.1532553517999998E-9</v>
+      </c>
+      <c r="L5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="59">
+        <v>11</v>
+      </c>
+      <c r="B6" s="59">
+        <v>116830622</v>
+      </c>
+      <c r="C6" s="60">
+        <v>116830927</v>
+      </c>
+      <c r="D6" s="59">
+        <v>57</v>
+      </c>
+      <c r="E6" s="81" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="82" t="s">
+        <v>505</v>
+      </c>
+      <c r="G6" s="85">
+        <v>2.11988808181599</v>
+      </c>
+      <c r="H6">
+        <v>0.95819310406795499</v>
+      </c>
+      <c r="I6" s="88">
+        <v>2.6940360373706802E-2</v>
+      </c>
+      <c r="J6" s="2">
+        <v>47</v>
+      </c>
+      <c r="K6" s="23">
+        <v>1.37667655053519E-14</v>
+      </c>
+      <c r="L6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="59">
+        <v>9</v>
+      </c>
+      <c r="B7" s="59">
+        <v>104858320</v>
+      </c>
+      <c r="C7" s="60">
+        <v>104858572</v>
+      </c>
+      <c r="D7" s="59">
+        <v>39</v>
+      </c>
+      <c r="E7" s="81" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="82" t="s">
+        <v>506</v>
+      </c>
+      <c r="G7" s="85">
+        <v>-3.4417798210556199</v>
+      </c>
+      <c r="H7">
+        <v>0.90942132421060995</v>
+      </c>
+      <c r="I7" s="88">
+        <v>1.53966969356265E-4</v>
+      </c>
+      <c r="J7" s="2">
+        <v>42</v>
+      </c>
+      <c r="K7" s="23">
+        <v>4.8120045106058301E-23</v>
+      </c>
+      <c r="L7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="59">
+        <v>9</v>
+      </c>
+      <c r="B8" s="59">
+        <v>104858238</v>
+      </c>
+      <c r="C8" s="60">
+        <v>104858595</v>
+      </c>
+      <c r="D8" s="59">
+        <v>59</v>
+      </c>
+      <c r="E8" s="81" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="82" t="s">
+        <v>507</v>
+      </c>
+      <c r="G8" s="85">
+        <v>-0.38737831479964102</v>
+      </c>
+      <c r="H8">
+        <v>0.50129389215267695</v>
+      </c>
+      <c r="I8" s="88">
+        <v>0.43966626431274503</v>
+      </c>
+      <c r="J8" s="2">
+        <v>56</v>
+      </c>
+      <c r="K8" s="23">
+        <v>2.6149963464964698E-22</v>
+      </c>
+      <c r="L8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="59">
+        <v>16</v>
+      </c>
+      <c r="B9" s="59">
+        <v>57053861</v>
+      </c>
+      <c r="C9" s="60">
+        <v>57055228</v>
+      </c>
+      <c r="D9" s="59">
+        <v>200</v>
+      </c>
+      <c r="E9" s="81" t="s">
+        <v>404</v>
+      </c>
+      <c r="F9" s="82" t="s">
+        <v>508</v>
+      </c>
+      <c r="G9" s="85">
+        <v>-2.1182793086156502</v>
+      </c>
+      <c r="H9">
+        <v>0.25062973247325498</v>
+      </c>
+      <c r="I9" s="88">
+        <v>2.8677767028151397E-17</v>
+      </c>
+      <c r="J9" s="2">
+        <v>198</v>
+      </c>
+      <c r="K9" s="23">
+        <v>2.12427978937768E-2</v>
+      </c>
+      <c r="L9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="59">
+        <v>8</v>
+      </c>
+      <c r="B10" s="59">
+        <v>19973249</v>
+      </c>
+      <c r="C10" s="60">
+        <v>19973838</v>
+      </c>
+      <c r="D10" s="59">
+        <v>120</v>
+      </c>
+      <c r="E10" s="81" t="s">
+        <v>509</v>
+      </c>
+      <c r="F10" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="85">
+        <v>1.89884835402314</v>
+      </c>
+      <c r="H10">
+        <v>0.29322972274133502</v>
+      </c>
+      <c r="I10" s="88">
+        <v>9.4414672068534404E-11</v>
+      </c>
+      <c r="J10" s="2">
+        <v>94</v>
+      </c>
+      <c r="K10" s="23">
+        <v>1.45266706345515E-4</v>
+      </c>
+      <c r="L10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="59">
+        <v>7</v>
+      </c>
+      <c r="B11" s="59">
+        <v>80590516</v>
+      </c>
+      <c r="C11" s="60">
+        <v>80592668</v>
+      </c>
+      <c r="D11" s="59">
+        <v>279</v>
+      </c>
+      <c r="E11" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="60" t="s">
+        <v>510</v>
+      </c>
+      <c r="G11" s="85">
+        <v>-0.26506478076173101</v>
+      </c>
+      <c r="H11">
+        <v>0.21614730801409501</v>
+      </c>
+      <c r="I11" s="88">
+        <v>0.220079993899539</v>
+      </c>
+      <c r="J11" s="2">
+        <v>294</v>
+      </c>
+      <c r="K11" s="23">
+        <v>2.3585970433040001E-2</v>
+      </c>
+      <c r="L11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="62" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="67">
+        <v>16</v>
+      </c>
+      <c r="B12" s="67">
+        <v>67942882</v>
+      </c>
+      <c r="C12" s="68">
+        <v>67943605</v>
+      </c>
+      <c r="D12" s="67">
+        <v>109</v>
+      </c>
+      <c r="E12" s="83" t="s">
+        <v>511</v>
+      </c>
+      <c r="F12" s="68" t="s">
+        <v>512</v>
+      </c>
+      <c r="G12" s="86">
+        <v>0.73115733991596898</v>
+      </c>
+      <c r="H12">
+        <v>0.52174357865867205</v>
+      </c>
+      <c r="I12" s="89">
+        <v>0.16110257570900699</v>
+      </c>
+      <c r="J12" s="33">
+        <v>108</v>
+      </c>
+      <c r="K12" s="28">
+        <v>2.51455086190191E-23</v>
+      </c>
+      <c r="L12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>